<commit_message>
remove inactive in summary export. remove reffered
</commit_message>
<xml_diff>
--- a/public/template/Import_Record_Template.xlsx
+++ b/public/template/Import_Record_Template.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Nov 19 2020 - Dec 1 2020" sheetId="1" r:id="rId1"/>
     <sheet name="Dec 02 2020 - Dec 15 2020" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nov 19 2020 - Dec 1 2020'!$D$1:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nov 19 2020 - Dec 1 2020'!$D$1:$L$3</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t xml:space="preserve">ABAD, NELMA BORNEL </t>
   </si>
@@ -55,9 +55,6 @@
     <t>Requesting_Physician</t>
   </si>
   <si>
-    <t>Reffered_Physician</t>
-  </si>
-  <si>
     <t>Anesthesiology_Physician</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">  VolKmaN,  Orland  Ratke, Streich, Austyn GlovEr</t>
-  </si>
-  <si>
-    <t>Schamberger, Ahmad Bailey</t>
   </si>
   <si>
     <t>VolKman,  Orland  Ratke, Streich, Austyn Glover</t>
@@ -508,11 +502,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,16 +518,15 @@
     <col min="5" max="5" width="46.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -556,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>11</v>
@@ -573,11 +566,8 @@
       <c r="M1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,16 +581,16 @@
         <v>9700</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -614,14 +604,11 @@
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -635,7 +622,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
@@ -658,10 +645,7 @@
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -673,10 +657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,16 +672,15 @@
     <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -720,10 +703,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>11</v>
@@ -737,11 +720,8 @@
       <c r="M1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -755,16 +735,16 @@
         <v>9700</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -778,14 +758,11 @@
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +776,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
@@ -822,10 +799,7 @@
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reconstruct import export (#54)
* remove inactive in summary export. remove reffered

* uniform error message doctor component

* fix continue append data in export

* add doctor view patient

* remove unnecessary code
</commit_message>
<xml_diff>
--- a/public/template/Import_Record_Template.xlsx
+++ b/public/template/Import_Record_Template.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Nov 19 2020 - Dec 1 2020" sheetId="1" r:id="rId1"/>
     <sheet name="Dec 02 2020 - Dec 15 2020" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nov 19 2020 - Dec 1 2020'!$D$1:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nov 19 2020 - Dec 1 2020'!$D$1:$L$3</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t xml:space="preserve">ABAD, NELMA BORNEL </t>
   </si>
@@ -55,9 +55,6 @@
     <t>Requesting_Physician</t>
   </si>
   <si>
-    <t>Reffered_Physician</t>
-  </si>
-  <si>
     <t>Anesthesiology_Physician</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">  VolKmaN,  Orland  Ratke, Streich, Austyn GlovEr</t>
-  </si>
-  <si>
-    <t>Schamberger, Ahmad Bailey</t>
   </si>
   <si>
     <t>VolKman,  Orland  Ratke, Streich, Austyn Glover</t>
@@ -508,11 +502,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,16 +518,15 @@
     <col min="5" max="5" width="46.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -556,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>11</v>
@@ -573,11 +566,8 @@
       <c r="M1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,16 +581,16 @@
         <v>9700</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -614,14 +604,11 @@
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -635,7 +622,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
@@ -658,10 +645,7 @@
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -673,10 +657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,16 +672,15 @@
     <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -720,10 +703,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>11</v>
@@ -737,11 +720,8 @@
       <c r="M1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -755,16 +735,16 @@
         <v>9700</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -778,14 +758,11 @@
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +776,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
@@ -822,10 +799,7 @@
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Find bugs summary (#57)
* change view table for doctor summary

* filtered doctor summary by record id

* add doctor_record preview

* cotinue working on doctor summary

* shorten

* added grand total

* comply with travis 1

* comply with travis 2

* remove duplicate call class

Co-authored-by: MarkDy2797 <markdy61@gmail.com>
</commit_message>
<xml_diff>
--- a/public/template/Import_Record_Template.xlsx
+++ b/public/template/Import_Record_Template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SPICTD\SorPhilHealthSystem\public\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745" activeTab="1"/>
   </bookViews>
@@ -23,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
   <si>
     <t xml:space="preserve">ABAD, NELMA BORNEL </t>
   </si>
@@ -83,13 +78,16 @@
   </si>
   <si>
     <t>VolKman,  Orland  Ratke, Streich, Austyn Glover</t>
+  </si>
+  <si>
+    <t>Anesthesiologist_Physician</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,14 +492,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -509,7 +507,7 @@
       <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="5" customWidth="1"/>
@@ -526,7 +524,7 @@
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="8" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -567,7 +565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -656,14 +654,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
@@ -680,7 +678,7 @@
     <col min="13" max="13" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -706,7 +704,7 @@
         <v>15</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>11</v>
@@ -721,7 +719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -762,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Doctor record export (#58)
* fix doctor view patient

* add dynamic setting

* hide sidebar overflow x

* Merge branch 'development' of https://github.com/snretuerma/SorPhilHealthSystem into doctor_record_export

* shorten condition and add initial export

* finalize output

* comply with travis 1

* comply with travis 2

* reduce duplicate condition

* remove space

* delete message

* add active inactive doctor view

* fix restore

* fix restore
</commit_message>
<xml_diff>
--- a/public/template/Import_Record_Template.xlsx
+++ b/public/template/Import_Record_Template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SPICTD\SorPhilHealthSystem\public\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745"/>
   </bookViews>
   <sheets>
     <sheet name="Nov 19 2020 - Dec 1 2020" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t xml:space="preserve">ABAD, NELMA BORNEL </t>
   </si>
@@ -48,9 +53,6 @@
   </si>
   <si>
     <t>Requesting_Physician</t>
-  </si>
-  <si>
-    <t>Anesthesiology_Physician</t>
   </si>
   <si>
     <t>Surgeon_Physician</t>
@@ -86,8 +88,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,22 +494,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="5" customWidth="1"/>
@@ -524,7 +526,7 @@
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -547,25 +549,25 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -579,10 +581,10 @@
         <v>9700</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -606,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -620,7 +622,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
@@ -654,14 +656,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
@@ -678,7 +680,7 @@
     <col min="13" max="13" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -701,25 +703,25 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -733,10 +735,10 @@
         <v>9700</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -760,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -774,7 +776,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>

</xml_diff>